<commit_message>
All task till 12-Dec-2020 11:43am
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -157,11 +157,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -636,6 +636,7 @@
       <c r="C13" s="11"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="jFhRzv7Od1hoe3Ei//l027s/YkVHA/cjQ1Cg3emRHRei7PaMd+kvL4lwLArq/l07zHEJLDu0ns0XsAtNSyJ4tw==" saltValue="k6u3i6CCbWvjOP2An2WMJA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
All task till 12-Dec-2020 04:00 pm
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -173,7 +173,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,7 +483,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,25 +594,25 @@
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="16">
         <v>1</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="10">
         <v>44175</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="10">
         <v>44175</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="1"/>
@@ -636,7 +636,7 @@
       <c r="C13" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jFhRzv7Od1hoe3Ei//l027s/YkVHA/cjQ1Cg3emRHRei7PaMd+kvL4lwLArq/l07zHEJLDu0ns0XsAtNSyJ4tw==" saltValue="k6u3i6CCbWvjOP2An2WMJA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
All task till 19-Dec-2020 10:48 pm
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Java and DB Task</t>
   </si>
   <si>
-    <t>8k</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Dilivered</t>
   </si>
   <si>
-    <t>In  Progress</t>
-  </si>
-  <si>
     <t>Java Thred Task</t>
   </si>
   <si>
@@ -80,6 +74,24 @@
   </si>
   <si>
     <t>1k</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>9k</t>
+  </si>
+  <si>
+    <t>Canceled Task</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>7k</t>
+  </si>
+  <si>
+    <t>Database for Ticket System</t>
   </si>
 </sst>
 </file>
@@ -112,7 +124,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,31 +168,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,12 +524,12 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -498,106 +539,106 @@
     <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>44172</v>
+      </c>
+      <c r="D2" s="5">
+        <v>44173</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>44173</v>
+      </c>
+      <c r="D3" s="5">
+        <v>44180</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
-        <v>44172</v>
-      </c>
-      <c r="D2" s="6">
-        <v>44173</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="C4" s="5">
+        <v>44174</v>
+      </c>
+      <c r="D4" s="5">
+        <v>44174</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8">
-        <v>44173</v>
-      </c>
-      <c r="D3" s="8">
-        <v>44180</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10">
-        <v>44174</v>
-      </c>
-      <c r="D4" s="10">
-        <v>44174</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9">
         <v>1</v>
       </c>
       <c r="C5" s="10">
@@ -606,34 +647,61 @@
       <c r="D5" s="10">
         <v>44175</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="15" t="s">
+      <c r="E5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="16">
+        <v>7</v>
+      </c>
+      <c r="C6" s="17">
+        <v>44184</v>
+      </c>
+      <c r="D6" s="17">
+        <v>44190</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="15"/>
+      <c r="J7" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I6" s="3"/>
-      <c r="J6" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="2"/>
-      <c r="J7" s="15" t="s">
-        <v>18</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+      <c r="J8" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="11"/>
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
All task till 25-Dec-2020 07:38 pm
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -43,9 +43,6 @@
     <t>Java and DB Task</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Work Status</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Database for Ticket System</t>
+  </si>
+  <si>
+    <t>Delivered</t>
   </si>
 </sst>
 </file>
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,12 +209,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -524,7 +518,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -553,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -576,7 +570,7 @@
         <v>44173</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -600,10 +594,10 @@
         <v>44180</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>7</v>
@@ -612,7 +606,7 @@
     </row>
     <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -624,10 +618,10 @@
         <v>44174</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>7</v>
@@ -636,7 +630,7 @@
     </row>
     <row r="5" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -648,56 +642,56 @@
         <v>44175</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="14">
+        <v>7</v>
+      </c>
+      <c r="C6" s="14">
+        <v>44184</v>
+      </c>
+      <c r="D6" s="14">
+        <v>44190</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="16">
-        <v>7</v>
-      </c>
-      <c r="C6" s="17">
-        <v>44184</v>
-      </c>
-      <c r="D6" s="17">
-        <v>44190</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>9</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I7" s="15"/>
       <c r="J7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I8" s="3"/>
       <c r="J8" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All task till 27-Dec-2020 07:52 pm
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Description</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Paymnet</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Excel and DB Task</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Canceled Task</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>7k</t>
   </si>
   <si>
@@ -92,6 +86,15 @@
   </si>
   <si>
     <t>Delivered</t>
+  </si>
+  <si>
+    <t>Excel to Access Conversion</t>
+  </si>
+  <si>
+    <t>Payment Status</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,6 +212,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -518,7 +527,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +538,7 @@
     <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
     <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -538,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -547,18 +557,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -570,19 +580,19 @@
         <v>44173</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>7</v>
@@ -594,19 +604,19 @@
         <v>44180</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -618,19 +628,19 @@
         <v>44174</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -642,56 +652,79 @@
         <v>44175</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="14">
+      <c r="A6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="12">
         <v>7</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="5">
         <v>44184</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="5">
         <v>44190</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>25</v>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16">
+        <f ca="1">TODAY()</f>
+        <v>44192</v>
+      </c>
+      <c r="D7" s="16">
+        <f ca="1">TODAY()</f>
+        <v>44192</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="I7" s="15"/>
       <c r="J7" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I8" s="3"/>
       <c r="J8" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All task till 30-Dec-2020 07:49 pm
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Payment Status</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -171,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -212,12 +209,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,15 +518,14 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -693,28 +683,28 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="5">
         <f ca="1">TODAY()</f>
-        <v>44192</v>
-      </c>
-      <c r="D7" s="16">
+        <v>44195</v>
+      </c>
+      <c r="D7" s="5">
         <f ca="1">TODAY()</f>
-        <v>44192</v>
-      </c>
-      <c r="E7" s="17" t="s">
+        <v>44195</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>26</v>
+      <c r="G7" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="13" t="s">

</xml_diff>

<commit_message>
All Tasks Till 05-Jan-2021
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Description</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Payment Status</t>
+  </si>
+  <si>
+    <t>DataBase Task</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>8k</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +131,14 @@
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -168,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,6 +226,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -518,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,12 +716,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="5">
-        <f ca="1">TODAY()</f>
-        <v>44195</v>
+        <v>44184</v>
       </c>
       <c r="D7" s="5">
-        <f ca="1">TODAY()</f>
-        <v>44195</v>
+        <v>44184</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
@@ -717,11 +741,47 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="16">
+        <v>2021</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="17">
+        <v>44201</v>
+      </c>
+      <c r="D11" s="17">
+        <v>44201</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="C9:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
All Tasks Till 08-Jan-2021
</commit_message>
<xml_diff>
--- a/Tasks Details.xlsx
+++ b/Tasks Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -94,13 +94,10 @@
     <t>Payment Status</t>
   </si>
   <si>
-    <t>DataBase Task</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>8k</t>
+  </si>
+  <si>
+    <t>DataBase Task (Waleed)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -229,12 +226,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,7 +535,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,26 +743,26 @@
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>44201</v>
+      </c>
+      <c r="D11" s="5">
+        <v>44201</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="14">
-        <v>1</v>
-      </c>
-      <c r="C11" s="17">
-        <v>44201</v>
-      </c>
-      <c r="D11" s="17">
-        <v>44201</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>27</v>
+      <c r="G11" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>